<commit_message>
change hostname; add related indicator
change 'hostName' to 'domainName'; add a related Indicators tag that
points from one file to another; prettyize; add 'blobs' to discuss
examples.
</commit_message>
<xml_diff>
--- a/stix/scans/stix_scanning_for_user_profile.xlsx
+++ b/stix/scans/stix_scanning_for_user_profile.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="104">
   <si>
     <t>Profile Information</t>
   </si>
@@ -327,6 +327,9 @@
   <si>
     <t>defaults to '99 - No Restrictions'</t>
   </si>
+  <si>
+    <t>domain_name-UUID4 format</t>
+  </si>
 </sst>
 </file>
 
@@ -553,7 +556,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="32">
     <dxf>
       <font>
         <sz val="11"/>
@@ -938,102 +941,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF16365C"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF95B3D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C6500"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006100"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF16365C"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF95B3D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1333,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34420,6 +34327,9 @@
       <c r="B39" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D39" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
@@ -34489,7 +34399,7 @@
         <v>60</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>